<commit_message>
add document for html pc
</commit_message>
<xml_diff>
--- a/documents/税聚java进度1014.xlsx
+++ b/documents/税聚java进度1014.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IBM_ADMIN\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rex\personal\git\taxparty\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="147">
   <si>
     <t>项目开发评估计划</t>
   </si>
@@ -177,9 +177,6 @@
     <t>有问题</t>
   </si>
   <si>
-    <t>修改中</t>
-  </si>
-  <si>
     <t>税务大咖选择</t>
   </si>
   <si>
@@ -216,9 +213,6 @@
     <t>问题分享</t>
   </si>
   <si>
-    <t>前端插件</t>
-  </si>
-  <si>
     <t>低优先级</t>
   </si>
   <si>
@@ -466,6 +460,9 @@
   </si>
   <si>
     <t>等待确认需求</t>
+  </si>
+  <si>
+    <t>正在联调</t>
   </si>
 </sst>
 </file>
@@ -826,26 +823,32 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -856,24 +859,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -895,13 +880,25 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1279,8 +1276,8 @@
   <dimension ref="A1:N85"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H72" sqref="H72"/>
+      <pane ySplit="3" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G48" sqref="G48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.42578125" defaultRowHeight="15"/>
@@ -1297,31 +1294,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="40.5" customHeight="1">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="60"/>
+      <c r="H1" s="60"/>
+      <c r="I1" s="60"/>
       <c r="J1" s="28"/>
       <c r="K1" s="6"/>
       <c r="L1" s="29"/>
     </row>
     <row r="2" spans="1:14" s="1" customFormat="1" ht="26.25">
-      <c r="A2" s="42" t="s">
+      <c r="A2" s="61" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
+      <c r="B2" s="62"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
+      <c r="G2" s="62"/>
       <c r="H2" s="7"/>
       <c r="I2" s="7"/>
       <c r="J2" s="30"/>
@@ -1364,9 +1361,9 @@
       <c r="K3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="L3" s="44"/>
-      <c r="M3" s="45"/>
-      <c r="N3" s="46"/>
+      <c r="L3" s="63"/>
+      <c r="M3" s="64"/>
+      <c r="N3" s="65"/>
     </row>
     <row r="4" spans="1:14" s="1" customFormat="1" ht="19.5" customHeight="1">
       <c r="A4" s="8" t="s">
@@ -1392,7 +1389,7 @@
       </c>
     </row>
     <row r="5" spans="1:14" s="1" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A5" s="47" t="s">
+      <c r="A5" s="49" t="s">
         <v>17</v>
       </c>
       <c r="B5" s="8" t="s">
@@ -1415,8 +1412,8 @@
       </c>
     </row>
     <row r="6" spans="1:14" s="1" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A6" s="48"/>
-      <c r="B6" s="47" t="s">
+      <c r="A6" s="50"/>
+      <c r="B6" s="49" t="s">
         <v>18</v>
       </c>
       <c r="C6" s="14" t="s">
@@ -1439,8 +1436,8 @@
       </c>
     </row>
     <row r="7" spans="1:14" s="1" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A7" s="48"/>
-      <c r="B7" s="48"/>
+      <c r="A7" s="50"/>
+      <c r="B7" s="50"/>
       <c r="C7" s="14" t="s">
         <v>21</v>
       </c>
@@ -1461,8 +1458,8 @@
       </c>
     </row>
     <row r="8" spans="1:14" s="1" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A8" s="48"/>
-      <c r="B8" s="48"/>
+      <c r="A8" s="50"/>
+      <c r="B8" s="50"/>
       <c r="C8" s="14" t="s">
         <v>23</v>
       </c>
@@ -1483,8 +1480,8 @@
       </c>
     </row>
     <row r="9" spans="1:14" s="1" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A9" s="48"/>
-      <c r="B9" s="48"/>
+      <c r="A9" s="50"/>
+      <c r="B9" s="50"/>
       <c r="C9" s="14" t="s">
         <v>24</v>
       </c>
@@ -1505,8 +1502,8 @@
       </c>
     </row>
     <row r="10" spans="1:14" s="1" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A10" s="49"/>
-      <c r="B10" s="49"/>
+      <c r="A10" s="51"/>
+      <c r="B10" s="51"/>
       <c r="C10" s="14" t="s">
         <v>25</v>
       </c>
@@ -1527,7 +1524,7 @@
       </c>
     </row>
     <row r="11" spans="1:14" s="1" customFormat="1">
-      <c r="A11" s="47" t="s">
+      <c r="A11" s="49" t="s">
         <v>26</v>
       </c>
       <c r="B11" s="8" t="s">
@@ -1550,7 +1547,7 @@
       </c>
     </row>
     <row r="12" spans="1:14" s="1" customFormat="1">
-      <c r="A12" s="49"/>
+      <c r="A12" s="51"/>
       <c r="B12" s="8" t="s">
         <v>29</v>
       </c>
@@ -1571,7 +1568,7 @@
       </c>
     </row>
     <row r="13" spans="1:14" s="1" customFormat="1">
-      <c r="A13" s="47" t="s">
+      <c r="A13" s="49" t="s">
         <v>30</v>
       </c>
       <c r="B13" s="8" t="s">
@@ -1590,7 +1587,7 @@
       </c>
     </row>
     <row r="14" spans="1:14" s="1" customFormat="1">
-      <c r="A14" s="48"/>
+      <c r="A14" s="50"/>
       <c r="B14" s="8" t="s">
         <v>33</v>
       </c>
@@ -1607,7 +1604,7 @@
       </c>
     </row>
     <row r="15" spans="1:14" s="1" customFormat="1">
-      <c r="A15" s="48"/>
+      <c r="A15" s="50"/>
       <c r="B15" s="8" t="s">
         <v>34</v>
       </c>
@@ -1624,7 +1621,7 @@
       </c>
     </row>
     <row r="16" spans="1:14" s="1" customFormat="1">
-      <c r="A16" s="49"/>
+      <c r="A16" s="51"/>
       <c r="B16" s="8" t="s">
         <v>35</v>
       </c>
@@ -1641,7 +1638,7 @@
       </c>
     </row>
     <row r="17" spans="1:11">
-      <c r="A17" s="50" t="s">
+      <c r="A17" s="43" t="s">
         <v>36</v>
       </c>
       <c r="B17" s="17" t="s">
@@ -1660,7 +1657,7 @@
       </c>
     </row>
     <row r="18" spans="1:11">
-      <c r="A18" s="51"/>
+      <c r="A18" s="44"/>
       <c r="B18" s="17" t="s">
         <v>38</v>
       </c>
@@ -1677,7 +1674,7 @@
       </c>
     </row>
     <row r="19" spans="1:11">
-      <c r="A19" s="51"/>
+      <c r="A19" s="44"/>
       <c r="B19" s="17" t="s">
         <v>40</v>
       </c>
@@ -1694,7 +1691,7 @@
       </c>
     </row>
     <row r="20" spans="1:11">
-      <c r="A20" s="51"/>
+      <c r="A20" s="44"/>
       <c r="B20" s="17" t="s">
         <v>41</v>
       </c>
@@ -1711,7 +1708,7 @@
       </c>
     </row>
     <row r="21" spans="1:11">
-      <c r="A21" s="52"/>
+      <c r="A21" s="45"/>
       <c r="B21" s="17" t="s">
         <v>42</v>
       </c>
@@ -1747,10 +1744,10 @@
       </c>
     </row>
     <row r="23" spans="1:11">
-      <c r="A23" s="53" t="s">
+      <c r="A23" s="46" t="s">
         <v>44</v>
       </c>
-      <c r="B23" s="56" t="s">
+      <c r="B23" s="52" t="s">
         <v>45</v>
       </c>
       <c r="C23" s="17" t="s">
@@ -1759,17 +1756,17 @@
       <c r="D23" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="E23" s="50" t="s">
+      <c r="E23" s="43" t="s">
         <v>48</v>
       </c>
-      <c r="F23" s="50" t="s">
+      <c r="F23" s="43" t="s">
         <v>49</v>
       </c>
       <c r="G23" s="22" t="s">
         <v>50</v>
       </c>
       <c r="H23" s="23" t="s">
-        <v>51</v>
+        <v>22</v>
       </c>
       <c r="I23" s="36" t="s">
         <v>32</v>
@@ -1782,21 +1779,21 @@
       </c>
     </row>
     <row r="24" spans="1:11">
-      <c r="A24" s="54"/>
-      <c r="B24" s="54"/>
+      <c r="A24" s="47"/>
+      <c r="B24" s="47"/>
       <c r="C24" s="17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D24" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="E24" s="51"/>
-      <c r="F24" s="51"/>
+      <c r="E24" s="44"/>
+      <c r="F24" s="44"/>
       <c r="G24" s="22" t="s">
         <v>50</v>
       </c>
       <c r="H24" s="24" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I24" s="36" t="s">
         <v>32</v>
@@ -1809,16 +1806,16 @@
       </c>
     </row>
     <row r="25" spans="1:11">
-      <c r="A25" s="54"/>
-      <c r="B25" s="54"/>
+      <c r="A25" s="47"/>
+      <c r="B25" s="47"/>
       <c r="C25" s="17" t="s">
         <v>45</v>
       </c>
       <c r="D25" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="E25" s="51"/>
-      <c r="F25" s="51"/>
+      <c r="E25" s="44"/>
+      <c r="F25" s="44"/>
       <c r="G25" s="19"/>
       <c r="I25" s="36" t="s">
         <v>32</v>
@@ -1831,16 +1828,16 @@
       </c>
     </row>
     <row r="26" spans="1:11">
-      <c r="A26" s="54"/>
-      <c r="B26" s="54"/>
+      <c r="A26" s="47"/>
+      <c r="B26" s="47"/>
       <c r="C26" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D26" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="E26" s="52"/>
-      <c r="F26" s="52"/>
+      <c r="E26" s="45"/>
+      <c r="F26" s="45"/>
       <c r="G26" s="20"/>
       <c r="I26" s="36" t="s">
         <v>32</v>
@@ -1853,10 +1850,10 @@
       </c>
     </row>
     <row r="27" spans="1:11">
-      <c r="A27" s="54"/>
-      <c r="B27" s="54"/>
+      <c r="A27" s="47"/>
+      <c r="B27" s="47"/>
       <c r="C27" s="17" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D27" s="21" t="s">
         <v>47</v>
@@ -1865,7 +1862,7 @@
         <v>48</v>
       </c>
       <c r="F27" s="25" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G27" s="25"/>
       <c r="I27" s="36" t="s">
@@ -1879,19 +1876,19 @@
       </c>
     </row>
     <row r="28" spans="1:11">
-      <c r="A28" s="54"/>
-      <c r="B28" s="55"/>
+      <c r="A28" s="47"/>
+      <c r="B28" s="48"/>
       <c r="C28" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="D28" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="E28" s="43" t="s">
+        <v>48</v>
+      </c>
+      <c r="F28" s="43" t="s">
         <v>57</v>
-      </c>
-      <c r="D28" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="E28" s="50" t="s">
-        <v>48</v>
-      </c>
-      <c r="F28" s="50" t="s">
-        <v>58</v>
       </c>
       <c r="G28" s="16"/>
       <c r="I28" s="36" t="s">
@@ -1905,20 +1902,20 @@
       </c>
     </row>
     <row r="29" spans="1:11" ht="15" customHeight="1">
-      <c r="A29" s="54"/>
-      <c r="B29" s="57" t="s">
+      <c r="A29" s="47"/>
+      <c r="B29" s="53" t="s">
+        <v>58</v>
+      </c>
+      <c r="C29" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="C29" s="17" t="s">
+      <c r="D29" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="E29" s="44"/>
+      <c r="F29" s="44"/>
+      <c r="G29" s="26" t="s">
         <v>60</v>
-      </c>
-      <c r="D29" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="E29" s="51"/>
-      <c r="F29" s="51"/>
-      <c r="G29" s="26" t="s">
-        <v>61</v>
       </c>
       <c r="H29" s="15"/>
       <c r="I29" s="36" t="s">
@@ -1932,18 +1929,18 @@
       </c>
     </row>
     <row r="30" spans="1:11">
-      <c r="A30" s="54"/>
-      <c r="B30" s="58"/>
+      <c r="A30" s="47"/>
+      <c r="B30" s="54"/>
       <c r="C30" s="17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D30" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="E30" s="51"/>
-      <c r="F30" s="51"/>
+      <c r="E30" s="44"/>
+      <c r="F30" s="44"/>
       <c r="G30" s="26" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H30" s="15"/>
       <c r="I30" s="36" t="s">
@@ -1957,21 +1954,21 @@
       </c>
     </row>
     <row r="31" spans="1:11">
-      <c r="A31" s="54"/>
-      <c r="B31" s="58"/>
+      <c r="A31" s="47"/>
+      <c r="B31" s="54"/>
       <c r="C31" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="D31" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="E31" s="44"/>
+      <c r="F31" s="44"/>
+      <c r="G31" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="H31" s="2" t="s">
         <v>63</v>
-      </c>
-      <c r="D31" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="E31" s="51"/>
-      <c r="F31" s="51"/>
-      <c r="G31" s="24" t="s">
-        <v>64</v>
-      </c>
-      <c r="H31" s="2" t="s">
-        <v>65</v>
       </c>
       <c r="I31" s="36" t="s">
         <v>28</v>
@@ -1981,18 +1978,18 @@
       </c>
     </row>
     <row r="32" spans="1:11">
-      <c r="A32" s="55"/>
-      <c r="B32" s="59"/>
+      <c r="A32" s="48"/>
+      <c r="B32" s="55"/>
       <c r="C32" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D32" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="E32" s="51"/>
-      <c r="F32" s="52"/>
+      <c r="E32" s="44"/>
+      <c r="F32" s="45"/>
       <c r="G32" s="26" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I32" s="36" t="s">
         <v>28</v>
@@ -2005,14 +2002,14 @@
       </c>
     </row>
     <row r="33" spans="1:11">
-      <c r="A33" s="53" t="s">
-        <v>66</v>
-      </c>
-      <c r="B33" s="53" t="s">
-        <v>66</v>
+      <c r="A33" s="46" t="s">
+        <v>64</v>
+      </c>
+      <c r="B33" s="46" t="s">
+        <v>64</v>
       </c>
       <c r="C33" s="17" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D33" s="21" t="s">
         <v>47</v>
@@ -2021,21 +2018,21 @@
         <v>48</v>
       </c>
       <c r="F33" s="25" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G33" s="25"/>
       <c r="I33" s="36" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="J33" s="37">
         <v>42670</v>
       </c>
     </row>
     <row r="34" spans="1:11">
-      <c r="A34" s="54"/>
-      <c r="B34" s="54"/>
+      <c r="A34" s="47"/>
+      <c r="B34" s="47"/>
       <c r="C34" s="17" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D34" s="21" t="s">
         <v>47</v>
@@ -2044,21 +2041,21 @@
         <v>48</v>
       </c>
       <c r="F34" s="25" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G34" s="25"/>
       <c r="I34" s="36" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="J34" s="37">
         <v>42670</v>
       </c>
     </row>
     <row r="35" spans="1:11">
-      <c r="A35" s="54"/>
-      <c r="B35" s="54"/>
+      <c r="A35" s="47"/>
+      <c r="B35" s="47"/>
       <c r="C35" s="17" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D35" s="21" t="s">
         <v>47</v>
@@ -2067,21 +2064,21 @@
         <v>48</v>
       </c>
       <c r="F35" s="25" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G35" s="25"/>
       <c r="I35" s="36" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="J35" s="37">
         <v>42670</v>
       </c>
     </row>
     <row r="36" spans="1:11">
-      <c r="A36" s="54"/>
-      <c r="B36" s="54"/>
+      <c r="A36" s="47"/>
+      <c r="B36" s="47"/>
       <c r="C36" s="17" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D36" s="21" t="s">
         <v>47</v>
@@ -2090,21 +2087,21 @@
         <v>48</v>
       </c>
       <c r="F36" s="25" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="G36" s="25"/>
       <c r="I36" s="36" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="J36" s="37">
         <v>42670</v>
       </c>
     </row>
     <row r="37" spans="1:11">
-      <c r="A37" s="54"/>
-      <c r="B37" s="54"/>
+      <c r="A37" s="47"/>
+      <c r="B37" s="47"/>
       <c r="C37" s="17" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D37" s="21" t="s">
         <v>47</v>
@@ -2113,21 +2110,21 @@
         <v>48</v>
       </c>
       <c r="F37" s="25" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G37" s="25"/>
       <c r="I37" s="36" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="J37" s="37">
         <v>42670</v>
       </c>
     </row>
     <row r="38" spans="1:11">
-      <c r="A38" s="54"/>
-      <c r="B38" s="54"/>
+      <c r="A38" s="47"/>
+      <c r="B38" s="47"/>
       <c r="C38" s="17" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D38" s="21" t="s">
         <v>47</v>
@@ -2136,21 +2133,21 @@
         <v>48</v>
       </c>
       <c r="F38" s="25" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G38" s="25"/>
       <c r="I38" s="36" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="J38" s="37">
         <v>42670</v>
       </c>
     </row>
     <row r="39" spans="1:11">
-      <c r="A39" s="54"/>
-      <c r="B39" s="55"/>
+      <c r="A39" s="47"/>
+      <c r="B39" s="48"/>
       <c r="C39" s="17" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D39" s="21" t="s">
         <v>47</v>
@@ -2159,32 +2156,32 @@
         <v>48</v>
       </c>
       <c r="F39" s="25" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G39" s="25"/>
       <c r="I39" s="36" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="J39" s="37">
         <v>42670</v>
       </c>
     </row>
     <row r="40" spans="1:11">
-      <c r="A40" s="54"/>
-      <c r="B40" s="53" t="s">
-        <v>81</v>
+      <c r="A40" s="47"/>
+      <c r="B40" s="46" t="s">
+        <v>79</v>
       </c>
       <c r="C40" s="17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D40" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="E40" s="51" t="s">
+      <c r="E40" s="44" t="s">
         <v>48</v>
       </c>
-      <c r="F40" s="50" t="s">
-        <v>82</v>
+      <c r="F40" s="43" t="s">
+        <v>80</v>
       </c>
       <c r="G40" s="16"/>
       <c r="I40" s="36" t="s">
@@ -2195,16 +2192,16 @@
       </c>
     </row>
     <row r="41" spans="1:11">
-      <c r="A41" s="54"/>
-      <c r="B41" s="54"/>
+      <c r="A41" s="47"/>
+      <c r="B41" s="47"/>
       <c r="C41" s="17" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D41" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="E41" s="51"/>
-      <c r="F41" s="51"/>
+      <c r="E41" s="44"/>
+      <c r="F41" s="44"/>
       <c r="G41" s="19"/>
       <c r="I41" s="36" t="s">
         <v>28</v>
@@ -2214,16 +2211,16 @@
       </c>
     </row>
     <row r="42" spans="1:11">
-      <c r="A42" s="55"/>
-      <c r="B42" s="55"/>
+      <c r="A42" s="48"/>
+      <c r="B42" s="48"/>
       <c r="C42" s="17" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D42" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="E42" s="52"/>
-      <c r="F42" s="51"/>
+      <c r="E42" s="45"/>
+      <c r="F42" s="44"/>
       <c r="G42" s="19"/>
       <c r="I42" s="36" t="s">
         <v>28</v>
@@ -2233,24 +2230,24 @@
       </c>
     </row>
     <row r="43" spans="1:11">
-      <c r="A43" s="53" t="s">
-        <v>85</v>
+      <c r="A43" s="46" t="s">
+        <v>83</v>
       </c>
       <c r="B43" s="17" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C43" s="17"/>
       <c r="D43" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="E43" s="50" t="s">
+      <c r="E43" s="43" t="s">
         <v>48</v>
       </c>
-      <c r="F43" s="50" t="s">
-        <v>87</v>
+      <c r="F43" s="43" t="s">
+        <v>85</v>
       </c>
       <c r="G43" s="26" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I43" s="36" t="s">
         <v>39</v>
@@ -2263,18 +2260,18 @@
       </c>
     </row>
     <row r="44" spans="1:11">
-      <c r="A44" s="54"/>
+      <c r="A44" s="47"/>
       <c r="B44" s="17" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C44" s="17"/>
       <c r="D44" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="E44" s="51"/>
-      <c r="F44" s="51"/>
+      <c r="E44" s="44"/>
+      <c r="F44" s="44"/>
       <c r="G44" s="26" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I44" s="36" t="s">
         <v>39</v>
@@ -2287,18 +2284,18 @@
       </c>
     </row>
     <row r="45" spans="1:11">
-      <c r="A45" s="54"/>
+      <c r="A45" s="47"/>
       <c r="B45" s="17" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C45" s="17"/>
       <c r="D45" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="E45" s="51"/>
-      <c r="F45" s="51"/>
+      <c r="E45" s="44"/>
+      <c r="F45" s="44"/>
       <c r="G45" s="26" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I45" s="36" t="s">
         <v>39</v>
@@ -2311,18 +2308,18 @@
       </c>
     </row>
     <row r="46" spans="1:11">
-      <c r="A46" s="54"/>
+      <c r="A46" s="47"/>
       <c r="B46" s="17" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C46" s="17"/>
       <c r="D46" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="E46" s="51"/>
-      <c r="F46" s="51"/>
+      <c r="E46" s="44"/>
+      <c r="F46" s="44"/>
       <c r="G46" s="26" t="s">
-        <v>61</v>
+        <v>146</v>
       </c>
       <c r="I46" s="36" t="s">
         <v>39</v>
@@ -2335,18 +2332,18 @@
       </c>
     </row>
     <row r="47" spans="1:11">
-      <c r="A47" s="54"/>
+      <c r="A47" s="47"/>
       <c r="B47" s="17" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C47" s="17"/>
       <c r="D47" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="E47" s="51"/>
-      <c r="F47" s="51"/>
+      <c r="E47" s="44"/>
+      <c r="F47" s="44"/>
       <c r="G47" s="26" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I47" s="36" t="s">
         <v>39</v>
@@ -2359,21 +2356,21 @@
       </c>
     </row>
     <row r="48" spans="1:11">
-      <c r="A48" s="54"/>
+      <c r="A48" s="47"/>
       <c r="B48" s="17" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C48" s="17"/>
       <c r="D48" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="E48" s="51"/>
-      <c r="F48" s="51"/>
-      <c r="G48" s="24" t="s">
-        <v>64</v>
+      <c r="E48" s="44"/>
+      <c r="F48" s="44"/>
+      <c r="G48" s="22" t="s">
+        <v>50</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I48" s="36" t="s">
         <v>39</v>
@@ -2386,18 +2383,18 @@
       </c>
     </row>
     <row r="49" spans="1:11">
-      <c r="A49" s="55"/>
+      <c r="A49" s="48"/>
       <c r="B49" s="17" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C49" s="17"/>
       <c r="D49" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="E49" s="52"/>
-      <c r="F49" s="52"/>
+      <c r="E49" s="45"/>
+      <c r="F49" s="45"/>
       <c r="G49" s="26" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I49" s="36" t="s">
         <v>39</v>
@@ -2410,14 +2407,14 @@
       </c>
     </row>
     <row r="50" spans="1:11">
-      <c r="A50" s="53" t="s">
+      <c r="A50" s="46" t="s">
+        <v>92</v>
+      </c>
+      <c r="B50" s="46" t="s">
+        <v>93</v>
+      </c>
+      <c r="C50" s="27" t="s">
         <v>94</v>
-      </c>
-      <c r="B50" s="53" t="s">
-        <v>95</v>
-      </c>
-      <c r="C50" s="27" t="s">
-        <v>96</v>
       </c>
       <c r="D50" s="2" t="s">
         <v>14</v>
@@ -2432,10 +2429,10 @@
       </c>
     </row>
     <row r="51" spans="1:11">
-      <c r="A51" s="54"/>
-      <c r="B51" s="54"/>
+      <c r="A51" s="47"/>
+      <c r="B51" s="47"/>
       <c r="C51" s="27" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D51" s="2" t="s">
         <v>14</v>
@@ -2450,10 +2447,10 @@
       </c>
     </row>
     <row r="52" spans="1:11">
-      <c r="A52" s="54"/>
-      <c r="B52" s="54"/>
+      <c r="A52" s="47"/>
+      <c r="B52" s="47"/>
       <c r="C52" s="27" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D52" s="2" t="s">
         <v>14</v>
@@ -2468,10 +2465,10 @@
       </c>
     </row>
     <row r="53" spans="1:11">
-      <c r="A53" s="54"/>
-      <c r="B53" s="54"/>
+      <c r="A53" s="47"/>
+      <c r="B53" s="47"/>
       <c r="C53" s="27" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D53" s="2" t="s">
         <v>14</v>
@@ -2486,10 +2483,10 @@
       </c>
     </row>
     <row r="54" spans="1:11">
-      <c r="A54" s="54"/>
-      <c r="B54" s="55"/>
+      <c r="A54" s="47"/>
+      <c r="B54" s="48"/>
       <c r="C54" s="27" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D54" s="2" t="s">
         <v>14</v>
@@ -2504,12 +2501,12 @@
       </c>
     </row>
     <row r="55" spans="1:11">
-      <c r="A55" s="54"/>
-      <c r="B55" s="53" t="s">
-        <v>101</v>
+      <c r="A55" s="47"/>
+      <c r="B55" s="46" t="s">
+        <v>99</v>
       </c>
       <c r="C55" s="27" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D55" s="2" t="s">
         <v>14</v>
@@ -2524,10 +2521,10 @@
       </c>
     </row>
     <row r="56" spans="1:11">
-      <c r="A56" s="54"/>
-      <c r="B56" s="55"/>
+      <c r="A56" s="47"/>
+      <c r="B56" s="48"/>
       <c r="C56" s="27" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D56" s="2" t="s">
         <v>14</v>
@@ -2542,12 +2539,12 @@
       </c>
     </row>
     <row r="57" spans="1:11">
-      <c r="A57" s="54"/>
-      <c r="B57" s="53" t="s">
-        <v>104</v>
+      <c r="A57" s="47"/>
+      <c r="B57" s="46" t="s">
+        <v>102</v>
       </c>
       <c r="C57" s="27" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D57" s="2" t="s">
         <v>14</v>
@@ -2562,10 +2559,10 @@
       </c>
     </row>
     <row r="58" spans="1:11">
-      <c r="A58" s="54"/>
-      <c r="B58" s="54"/>
+      <c r="A58" s="47"/>
+      <c r="B58" s="47"/>
       <c r="C58" s="27" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D58" s="2" t="s">
         <v>14</v>
@@ -2580,10 +2577,10 @@
       </c>
     </row>
     <row r="59" spans="1:11">
-      <c r="A59" s="54"/>
-      <c r="B59" s="55"/>
+      <c r="A59" s="47"/>
+      <c r="B59" s="48"/>
       <c r="C59" s="27" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D59" s="2" t="s">
         <v>14</v>
@@ -2598,24 +2595,24 @@
       </c>
     </row>
     <row r="60" spans="1:11">
-      <c r="A60" s="54"/>
-      <c r="B60" s="53" t="s">
+      <c r="A60" s="47"/>
+      <c r="B60" s="46" t="s">
         <v>44</v>
       </c>
       <c r="C60" s="27" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D60" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="E60" s="50" t="s">
+      <c r="E60" s="43" t="s">
         <v>48</v>
       </c>
-      <c r="F60" s="50" t="s">
-        <v>109</v>
+      <c r="F60" s="43" t="s">
+        <v>107</v>
       </c>
       <c r="G60" s="26" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I60" s="36" t="s">
         <v>32</v>
@@ -2625,18 +2622,18 @@
       </c>
     </row>
     <row r="61" spans="1:11">
-      <c r="A61" s="54"/>
-      <c r="B61" s="54"/>
+      <c r="A61" s="47"/>
+      <c r="B61" s="47"/>
       <c r="C61" s="27" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D61" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="E61" s="51"/>
-      <c r="F61" s="51"/>
+      <c r="E61" s="44"/>
+      <c r="F61" s="44"/>
       <c r="G61" s="26" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I61" s="36" t="s">
         <v>32</v>
@@ -2646,18 +2643,18 @@
       </c>
     </row>
     <row r="62" spans="1:11">
-      <c r="A62" s="54"/>
-      <c r="B62" s="54"/>
+      <c r="A62" s="47"/>
+      <c r="B62" s="47"/>
       <c r="C62" s="27" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D62" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="E62" s="51"/>
-      <c r="F62" s="51"/>
+      <c r="E62" s="44"/>
+      <c r="F62" s="44"/>
       <c r="G62" s="26" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I62" s="36" t="s">
         <v>32</v>
@@ -2667,18 +2664,18 @@
       </c>
     </row>
     <row r="63" spans="1:11">
-      <c r="A63" s="54"/>
-      <c r="B63" s="55"/>
+      <c r="A63" s="47"/>
+      <c r="B63" s="48"/>
       <c r="C63" s="27" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D63" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="E63" s="52"/>
-      <c r="F63" s="52"/>
+      <c r="E63" s="45"/>
+      <c r="F63" s="45"/>
       <c r="G63" s="26" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I63" s="36" t="s">
         <v>32</v>
@@ -2688,24 +2685,24 @@
       </c>
     </row>
     <row r="64" spans="1:11" s="1" customFormat="1">
-      <c r="A64" s="54"/>
-      <c r="B64" s="60" t="s">
+      <c r="A64" s="47"/>
+      <c r="B64" s="56" t="s">
+        <v>111</v>
+      </c>
+      <c r="C64" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="D64" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="E64" s="40" t="s">
+        <v>48</v>
+      </c>
+      <c r="F64" s="43" t="s">
         <v>113</v>
       </c>
-      <c r="C64" s="14" t="s">
-        <v>114</v>
-      </c>
-      <c r="D64" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="E64" s="63" t="s">
-        <v>48</v>
-      </c>
-      <c r="F64" s="50" t="s">
-        <v>115</v>
-      </c>
       <c r="G64" s="26" t="s">
-        <v>61</v>
+        <v>146</v>
       </c>
       <c r="I64" s="36" t="s">
         <v>20</v>
@@ -2715,18 +2712,18 @@
       </c>
     </row>
     <row r="65" spans="1:11" s="1" customFormat="1">
-      <c r="A65" s="54"/>
-      <c r="B65" s="61"/>
+      <c r="A65" s="47"/>
+      <c r="B65" s="57"/>
       <c r="C65" s="14" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D65" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="E65" s="64"/>
-      <c r="F65" s="51"/>
-      <c r="G65" s="24" t="s">
-        <v>16</v>
+      <c r="E65" s="41"/>
+      <c r="F65" s="44"/>
+      <c r="G65" s="26" t="s">
+        <v>146</v>
       </c>
       <c r="I65" s="36" t="s">
         <v>20</v>
@@ -2736,20 +2733,20 @@
       </c>
     </row>
     <row r="66" spans="1:11" s="1" customFormat="1">
-      <c r="A66" s="54"/>
-      <c r="B66" s="60" t="s">
-        <v>117</v>
+      <c r="A66" s="47"/>
+      <c r="B66" s="56" t="s">
+        <v>115</v>
       </c>
       <c r="C66" s="14" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D66" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="E66" s="64"/>
-      <c r="F66" s="51"/>
+      <c r="E66" s="41"/>
+      <c r="F66" s="44"/>
       <c r="G66" s="26" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I66" s="36" t="s">
         <v>28</v>
@@ -2759,21 +2756,21 @@
       </c>
     </row>
     <row r="67" spans="1:11" s="1" customFormat="1">
-      <c r="A67" s="54"/>
-      <c r="B67" s="62"/>
+      <c r="A67" s="47"/>
+      <c r="B67" s="58"/>
       <c r="C67" s="14" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D67" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="E67" s="64"/>
-      <c r="F67" s="51"/>
+      <c r="E67" s="41"/>
+      <c r="F67" s="44"/>
       <c r="G67" s="24" t="s">
         <v>16</v>
       </c>
       <c r="H67" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="I67" s="36" t="s">
         <v>28</v>
@@ -2783,21 +2780,21 @@
       </c>
     </row>
     <row r="68" spans="1:11" s="1" customFormat="1">
-      <c r="A68" s="54"/>
-      <c r="B68" s="61"/>
+      <c r="A68" s="47"/>
+      <c r="B68" s="57"/>
       <c r="C68" s="14" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D68" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="E68" s="65"/>
-      <c r="F68" s="52"/>
+      <c r="E68" s="42"/>
+      <c r="F68" s="45"/>
       <c r="G68" s="24" t="s">
         <v>16</v>
       </c>
       <c r="H68" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="I68" s="36" t="s">
         <v>28</v>
@@ -2807,12 +2804,12 @@
       </c>
     </row>
     <row r="69" spans="1:11" s="1" customFormat="1">
-      <c r="A69" s="54"/>
-      <c r="B69" s="60" t="s">
-        <v>121</v>
+      <c r="A69" s="47"/>
+      <c r="B69" s="56" t="s">
+        <v>119</v>
       </c>
       <c r="C69" s="14" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D69" s="21" t="s">
         <v>47</v>
@@ -2821,10 +2818,10 @@
         <v>48</v>
       </c>
       <c r="F69" s="25" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G69" s="26" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I69" s="36" t="s">
         <v>39</v>
@@ -2834,10 +2831,10 @@
       </c>
     </row>
     <row r="70" spans="1:11" s="1" customFormat="1">
-      <c r="A70" s="54"/>
-      <c r="B70" s="62"/>
+      <c r="A70" s="47"/>
+      <c r="B70" s="58"/>
       <c r="C70" s="14" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D70" s="21" t="s">
         <v>47</v>
@@ -2846,10 +2843,10 @@
         <v>48</v>
       </c>
       <c r="F70" s="25" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="G70" s="26" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I70" s="36" t="s">
         <v>39</v>
@@ -2859,10 +2856,10 @@
       </c>
     </row>
     <row r="71" spans="1:11" s="1" customFormat="1">
-      <c r="A71" s="54"/>
-      <c r="B71" s="62"/>
+      <c r="A71" s="47"/>
+      <c r="B71" s="58"/>
       <c r="C71" s="14" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D71" s="21" t="s">
         <v>47</v>
@@ -2871,13 +2868,13 @@
         <v>48</v>
       </c>
       <c r="F71" s="25" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G71" s="24" t="s">
         <v>16</v>
       </c>
       <c r="H71" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="I71" s="36" t="s">
         <v>39</v>
@@ -2887,10 +2884,10 @@
       </c>
     </row>
     <row r="72" spans="1:11" s="1" customFormat="1">
-      <c r="A72" s="54"/>
-      <c r="B72" s="61"/>
+      <c r="A72" s="47"/>
+      <c r="B72" s="57"/>
       <c r="C72" s="14" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D72" s="21" t="s">
         <v>47</v>
@@ -2899,13 +2896,13 @@
         <v>48</v>
       </c>
       <c r="F72" s="25" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="G72" s="24" t="s">
         <v>16</v>
       </c>
       <c r="H72" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="I72" s="36" t="s">
         <v>39</v>
@@ -2915,12 +2912,12 @@
       </c>
     </row>
     <row r="73" spans="1:11" s="1" customFormat="1">
-      <c r="A73" s="54"/>
-      <c r="B73" s="60" t="s">
-        <v>130</v>
+      <c r="A73" s="47"/>
+      <c r="B73" s="56" t="s">
+        <v>128</v>
       </c>
       <c r="C73" s="14" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D73" s="2" t="s">
         <v>14</v>
@@ -2935,10 +2932,10 @@
       </c>
     </row>
     <row r="74" spans="1:11" s="1" customFormat="1">
-      <c r="A74" s="54"/>
-      <c r="B74" s="61"/>
+      <c r="A74" s="47"/>
+      <c r="B74" s="57"/>
       <c r="C74" s="14" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D74" s="2" t="s">
         <v>14</v>
@@ -2953,12 +2950,12 @@
       </c>
     </row>
     <row r="75" spans="1:11" s="1" customFormat="1">
-      <c r="A75" s="54"/>
+      <c r="A75" s="47"/>
       <c r="B75" s="14" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C75" s="14" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D75" s="2" t="s">
         <v>14</v>
@@ -2973,12 +2970,12 @@
       </c>
     </row>
     <row r="76" spans="1:11" s="1" customFormat="1">
-      <c r="A76" s="54"/>
+      <c r="A76" s="47"/>
       <c r="B76" s="14" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C76" s="14" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D76" s="2" t="s">
         <v>14</v>
@@ -2993,12 +2990,12 @@
       </c>
     </row>
     <row r="77" spans="1:11" s="1" customFormat="1">
-      <c r="A77" s="54"/>
-      <c r="B77" s="60" t="s">
-        <v>135</v>
+      <c r="A77" s="47"/>
+      <c r="B77" s="56" t="s">
+        <v>133</v>
       </c>
       <c r="C77" s="14" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D77" s="2" t="s">
         <v>14</v>
@@ -3013,10 +3010,10 @@
       </c>
     </row>
     <row r="78" spans="1:11" s="1" customFormat="1">
-      <c r="A78" s="54"/>
-      <c r="B78" s="62"/>
+      <c r="A78" s="47"/>
+      <c r="B78" s="58"/>
       <c r="C78" s="14" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D78" s="2" t="s">
         <v>14</v>
@@ -3031,10 +3028,10 @@
       </c>
     </row>
     <row r="79" spans="1:11" s="1" customFormat="1">
-      <c r="A79" s="54"/>
-      <c r="B79" s="62"/>
+      <c r="A79" s="47"/>
+      <c r="B79" s="58"/>
       <c r="C79" s="14" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D79" s="2" t="s">
         <v>14</v>
@@ -3052,10 +3049,10 @@
       </c>
     </row>
     <row r="80" spans="1:11" s="1" customFormat="1">
-      <c r="A80" s="54"/>
-      <c r="B80" s="62"/>
+      <c r="A80" s="47"/>
+      <c r="B80" s="58"/>
       <c r="C80" s="14" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D80" s="2" t="s">
         <v>14</v>
@@ -3073,10 +3070,10 @@
       </c>
     </row>
     <row r="81" spans="1:11" s="1" customFormat="1">
-      <c r="A81" s="54"/>
-      <c r="B81" s="61"/>
+      <c r="A81" s="47"/>
+      <c r="B81" s="57"/>
       <c r="C81" s="14" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D81" s="2" t="s">
         <v>14</v>
@@ -3091,9 +3088,9 @@
       </c>
     </row>
     <row r="82" spans="1:11">
-      <c r="A82" s="55"/>
+      <c r="A82" s="48"/>
       <c r="B82" s="27" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D82" s="2" t="s">
         <v>14</v>
@@ -3107,41 +3104,38 @@
         <v>42657</v>
       </c>
       <c r="K82" s="39" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="83" spans="1:11">
       <c r="E83" s="2" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="J83" s="37"/>
     </row>
     <row r="84" spans="1:11">
       <c r="B84" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="J84" s="37"/>
     </row>
     <row r="85" spans="1:11">
       <c r="B85" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A3:K85"/>
   <mergeCells count="37">
-    <mergeCell ref="E64:E68"/>
-    <mergeCell ref="F23:F26"/>
-    <mergeCell ref="F28:F32"/>
-    <mergeCell ref="F40:F42"/>
-    <mergeCell ref="F43:F49"/>
-    <mergeCell ref="F60:F63"/>
-    <mergeCell ref="F64:F68"/>
-    <mergeCell ref="E23:E26"/>
-    <mergeCell ref="E28:E32"/>
-    <mergeCell ref="E40:E42"/>
-    <mergeCell ref="E43:E49"/>
-    <mergeCell ref="E60:E63"/>
+    <mergeCell ref="L3:N3"/>
+    <mergeCell ref="A5:A10"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="A17:A21"/>
+    <mergeCell ref="A23:A32"/>
+    <mergeCell ref="A33:A42"/>
+    <mergeCell ref="A43:A49"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:G2"/>
     <mergeCell ref="A50:A82"/>
     <mergeCell ref="B6:B10"/>
     <mergeCell ref="B23:B28"/>
@@ -3158,15 +3152,18 @@
     <mergeCell ref="B73:B74"/>
     <mergeCell ref="B77:B81"/>
     <mergeCell ref="A13:A16"/>
-    <mergeCell ref="A17:A21"/>
-    <mergeCell ref="A23:A32"/>
-    <mergeCell ref="A33:A42"/>
-    <mergeCell ref="A43:A49"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A2:G2"/>
-    <mergeCell ref="L3:N3"/>
-    <mergeCell ref="A5:A10"/>
-    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="E64:E68"/>
+    <mergeCell ref="F23:F26"/>
+    <mergeCell ref="F28:F32"/>
+    <mergeCell ref="F40:F42"/>
+    <mergeCell ref="F43:F49"/>
+    <mergeCell ref="F60:F63"/>
+    <mergeCell ref="F64:F68"/>
+    <mergeCell ref="E23:E26"/>
+    <mergeCell ref="E28:E32"/>
+    <mergeCell ref="E40:E42"/>
+    <mergeCell ref="E43:E49"/>
+    <mergeCell ref="E60:E63"/>
   </mergeCells>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>